<commit_message>
Kirstin: Added contribution percent, modified gitignore
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G12-9693-350-1261.xlsx
+++ b/Documentation/ProjectLog-G12-9693-350-1261.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KH/Documents/VSCodeProjects/ENSC_350/DP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE32EFC-FB26-2949-AA8F-7666692AF202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B6797A-7E20-EE47-B9FE-DE2B2C6F4CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="uphip+fyQmgTbQWVslgKndYGTCUT2nMCnU8pTyuiPxh9t3MkaNQeLeeV1eDZUH8uYM8JtsIZJzZApwnnbRUEcA==" workbookSaltValue="PVE5+bPUyqyV9jE5EaqSxw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="17380" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="26">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -418,6 +418,18 @@
   </si>
   <si>
     <t>G12</t>
+  </si>
+  <si>
+    <t>01/29/2026</t>
+  </si>
+  <si>
+    <t>01/31/2026</t>
+  </si>
+  <si>
+    <t>DP1.0: Refined table of contents, added boxes to each content rectangle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.0: Added subsections and content rectanges for conclusion section </t>
   </si>
 </sst>
 </file>
@@ -873,7 +885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -996,7 +1008,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="8" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1026,7 +1038,7 @@
     <xf numFmtId="18" fontId="5" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1050,7 +1062,11 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1443,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E6E40-83BD-4CBB-97D3-102021CD8368}">
   <dimension ref="A1:I783"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1476,7 +1492,7 @@
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="51"/>
@@ -1504,7 +1520,7 @@
       <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="56" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="42"/>
@@ -1517,8 +1533,8 @@
       <c r="A5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="41" t="s">
-        <v>12</v>
+      <c r="B5" s="41">
+        <v>0.33</v>
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="43"/>
@@ -1557,14 +1573,22 @@
       <c r="B7" s="12">
         <v>9693</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0.51388888888888884</v>
+      </c>
       <c r="F7" s="33"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="H7" s="11">
         <f t="shared" ref="H7" si="0">(E7-D7)*24</f>
-        <v>0</v>
+        <v>0.49999999999999822</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1573,28 +1597,34 @@
       <c r="B8" s="13">
         <v>9693</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="22"/>
+      <c r="C8" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="19">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="16"/>
+      <c r="G8" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="H8" s="26">
         <f>(E8-D8)*24</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
-      <c r="B9" s="13">
-        <v>9693</v>
-      </c>
+      <c r="B9" s="13"/>
       <c r="C9" s="21"/>
       <c r="D9" s="19"/>
       <c r="E9" s="22"/>
       <c r="F9" s="34"/>
       <c r="G9" s="16"/>
       <c r="H9" s="26">
-        <f t="shared" ref="H9:H72" si="1">(E9-D9)*24</f>
+        <f>(E9-D9)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -1607,7 +1637,7 @@
       <c r="F10" s="34"/>
       <c r="G10" s="16"/>
       <c r="H10" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H10:H72" si="1">(E10-D10)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -2512,7 +2542,7 @@
       <c r="F80" s="29"/>
       <c r="H80" s="28">
         <f>SUM(H7:H79)</f>
-        <v>0</v>
+        <v>3.4999999999999982</v>
       </c>
     </row>
     <row r="81" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3275,7 +3305,7 @@
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="51"/>
       <c r="D2" s="52"/>
       <c r="E2" s="44" t="s">
@@ -3299,7 +3329,7 @@
       <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="56" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="42"/>
@@ -3312,7 +3342,7 @@
       <c r="A5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="42"/>
@@ -5064,7 +5094,7 @@
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="51"/>
       <c r="D2" s="52"/>
       <c r="E2" s="44" t="s">
@@ -5088,7 +5118,7 @@
       <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="56" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="42"/>
@@ -5101,7 +5131,7 @@
       <c r="A5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="42"/>
@@ -6853,7 +6883,7 @@
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="51"/>
       <c r="D2" s="52"/>
       <c r="E2" s="44" t="s">
@@ -6877,7 +6907,7 @@
       <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="56" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="42"/>
@@ -6890,7 +6920,7 @@
       <c r="A5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="42"/>
@@ -8642,7 +8672,7 @@
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="51"/>
       <c r="D2" s="52"/>
       <c r="E2" s="44" t="s">
@@ -8666,7 +8696,7 @@
       <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="56" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="42"/>
@@ -8679,7 +8709,7 @@
       <c r="A5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="42"/>
@@ -10431,7 +10461,7 @@
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="51"/>
       <c r="D2" s="52"/>
       <c r="E2" s="44" t="s">
@@ -10455,7 +10485,7 @@
       <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="56" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="42"/>
@@ -10468,7 +10498,7 @@
       <c r="A5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="42"/>

</xml_diff>